<commit_message>
Fixed adjacency matrix and associated values.
</commit_message>
<xml_diff>
--- a/Closeness table.xlsx
+++ b/Closeness table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-37120" yWindow="-16620" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="10380" yWindow="0" windowWidth="15220" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -205,8 +205,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -246,15 +248,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -532,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:AL14"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AK2" sqref="AK2:AK14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -758,7 +762,7 @@
         <v>0</v>
       </c>
       <c r="AK2" s="5">
-        <v>0.219</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="AL2" s="5">
         <v>0.59199999999999997</v>
@@ -864,7 +868,7 @@
         <v>1</v>
       </c>
       <c r="AK3" s="5">
-        <v>0.3</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="AL3" s="5">
         <v>0.83799999999999997</v>
@@ -970,7 +974,7 @@
         <v>2</v>
       </c>
       <c r="AK4" s="5">
-        <v>0.3</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="AL4" s="5">
         <v>0.83799999999999997</v>
@@ -1076,7 +1080,7 @@
         <v>3</v>
       </c>
       <c r="AK5" s="5">
-        <v>0.3</v>
+        <v>0.316</v>
       </c>
       <c r="AL5" s="5">
         <v>0.94499999999999995</v>
@@ -1148,7 +1152,7 @@
         <v>0</v>
       </c>
       <c r="X6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y6" s="2">
         <v>0</v>
@@ -1182,7 +1186,7 @@
         <v>4</v>
       </c>
       <c r="AK6" s="5">
-        <v>0.219</v>
+        <v>0.33500000000000002</v>
       </c>
       <c r="AL6" s="5">
         <v>1</v>
@@ -1288,7 +1292,7 @@
         <v>5</v>
       </c>
       <c r="AK7" s="5">
-        <v>0.3</v>
+        <v>0.316</v>
       </c>
       <c r="AL7" s="5">
         <v>0.94499999999999995</v>
@@ -1394,7 +1398,7 @@
         <v>6</v>
       </c>
       <c r="AK8" s="5">
-        <v>0.3</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="AL8" s="5">
         <v>0.83799999999999997</v>
@@ -1500,7 +1504,7 @@
         <v>7</v>
       </c>
       <c r="AK9" s="5">
-        <v>0.219</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="AL9" s="5">
         <v>0.59199999999999997</v>
@@ -1606,7 +1610,7 @@
         <v>8</v>
       </c>
       <c r="AK10" s="5">
-        <v>0.3</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="AL10" s="5">
         <v>0.83799999999999997</v>
@@ -1712,7 +1716,7 @@
         <v>9</v>
       </c>
       <c r="AK11" s="5">
-        <v>0.3</v>
+        <v>0.316</v>
       </c>
       <c r="AL11" s="5">
         <v>0.94499999999999995</v>
@@ -1818,7 +1822,7 @@
         <v>10</v>
       </c>
       <c r="AK12" s="5">
-        <v>0.3</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="AL12" s="5">
         <v>0.83799999999999997</v>
@@ -1924,7 +1928,7 @@
         <v>11</v>
       </c>
       <c r="AK13" s="5">
-        <v>0.3</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="AL13" s="5">
         <v>0.83799999999999997</v>
@@ -2030,7 +2034,7 @@
         <v>12</v>
       </c>
       <c r="AK14" s="5">
-        <v>0.219</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="AL14" s="5">
         <v>0.59199999999999997</v>

</xml_diff>